<commit_message>
new sheet for analysis
</commit_message>
<xml_diff>
--- a/repos.xlsx
+++ b/repos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macleand/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jegoussc/Repositories/software_projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC04290C-8EE6-4741-AE11-67BC7FD9BC4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1415AF26-77EC-D94C-913C-E9A6C11AF97C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32120" yWindow="1920" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{CCCA6E0C-6F9D-4847-8935-3F469645A3E2}"/>
+    <workbookView xWindow="32120" yWindow="-6320" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{CCCA6E0C-6F9D-4847-8935-3F469645A3E2}"/>
   </bookViews>
   <sheets>
     <sheet name="software_tools" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="manuscripts" sheetId="3" r:id="rId3"/>
     <sheet name="tutorials" sheetId="2" r:id="rId4"/>
     <sheet name="pipelines" sheetId="4" r:id="rId5"/>
+    <sheet name="analysis" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="68">
   <si>
     <t>ena_scrape</t>
   </si>
@@ -230,6 +231,18 @@
   </si>
   <si>
     <t>https://github.com/TeamMacLean/hpc_download_documentation</t>
+  </si>
+  <si>
+    <t>lichens</t>
+  </si>
+  <si>
+    <t>Analysis of lichens transcription experiment data from the squamulose R package.</t>
+  </si>
+  <si>
+    <t>https://github.com/TeamMacLean/CJ_NT_1563_23_23022022_lichens/blob/main/README.md</t>
+  </si>
+  <si>
+    <t>clara</t>
   </si>
 </sst>
 </file>
@@ -836,8 +849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C6DDD31-3D0B-BB46-B206-37E6D0B2BD45}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1005,4 +1018,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86381A57-6E17-DB4E-9DDE-30C746BDBF0D}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>